<commit_message>
Finished up rough edges of the program
</commit_message>
<xml_diff>
--- a/DiscordChatExporter.Stats/template_stats.xlsx
+++ b/DiscordChatExporter.Stats/template_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christoph Tauchner\Desktop\Dateien\Freizeit\DiscordChatExporter\DiscordChatExporter.Stats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3CAE1AD-7F84-4E18-80FE-70E98869F02E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DFE749-3977-45B4-B506-BBE8A034380E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30840" yWindow="-540" windowWidth="30960" windowHeight="16920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WelcomeSheet" sheetId="4" r:id="rId1"/>
@@ -382,15 +382,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -417,6 +408,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4220,7 +4220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68B4B4C2-81DF-4215-BBB9-454D5A0480A0}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -4234,227 +4234,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="48" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="9"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="13"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="12" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="13"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="12" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="13"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="13"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="13"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="13" t="s">
+      <c r="D11" s="8"/>
+      <c r="E11" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="8"/>
+      <c r="C12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="13"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="13"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="13"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="13"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="13"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="13"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="13"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="13"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="19"/>
+      <c r="A23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -4844,7 +4844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{919CAE1E-ACA9-4548-8CAF-59D4047ED7DF}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>